<commit_message>
major feature update, including tag filters and logic to deal with API limits
</commit_message>
<xml_diff>
--- a/dynamo/DataEntryTemplate.xlsx
+++ b/dynamo/DataEntryTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjgleave/mysrc/aws-resource-group/dynamo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjgleave/mysrc/aws-tag-groups/dynamo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CED06755-785B-E64F-B9CF-A29E115761D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{61A2B037-B81C-9F4C-AC4C-8B3E764E24F4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="24100" windowHeight="14300" xr2:uid="{947D7F77-375C-4342-BF5A-F0821707019D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>BudgetCode</t>
   </si>
@@ -39,12 +39,6 @@
     <t>GroupValue</t>
   </si>
   <si>
-    <t>TagKey</t>
-  </si>
-  <si>
-    <t>TagValue</t>
-  </si>
-  <si>
     <t>EBSCostCenter</t>
   </si>
   <si>
@@ -60,15 +54,6 @@
     <t>SortKey</t>
   </si>
   <si>
-    <t>SecurityComponent</t>
-  </si>
-  <si>
-    <t>Identity</t>
-  </si>
-  <si>
-    <t>Threat</t>
-  </si>
-  <si>
     <t>TagGroup</t>
   </si>
   <si>
@@ -82,6 +67,48 @@
   </si>
   <si>
     <t>sec-threat</t>
+  </si>
+  <si>
+    <t>TagKey1</t>
+  </si>
+  <si>
+    <t>TagValue1</t>
+  </si>
+  <si>
+    <t>TagKey2</t>
+  </si>
+  <si>
+    <t>TagValue2</t>
+  </si>
+  <si>
+    <t>TagKey3</t>
+  </si>
+  <si>
+    <t>TagValue3</t>
+  </si>
+  <si>
+    <t>PROJECT-901233</t>
+  </si>
+  <si>
+    <t>PROJECT-896775</t>
+  </si>
+  <si>
+    <t>4000033</t>
+  </si>
+  <si>
+    <t>4000055</t>
+  </si>
+  <si>
+    <t>TagKey4</t>
+  </si>
+  <si>
+    <t>TagValue4</t>
+  </si>
+  <si>
+    <t>TagKey5</t>
+  </si>
+  <si>
+    <t>TagValue5</t>
   </si>
 </sst>
 </file>
@@ -437,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29527916-67E3-DC46-8A8F-3DD525A32FA1}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,131 +477,147 @@
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B7" si="0">A2&amp;"/"&amp;C2&amp;"/"&amp;D2&amp;"/"&amp;E2</f>
+        <f t="shared" ref="B2:B5" si="0">A2&amp;"/"&amp;C2&amp;"/"&amp;D2&amp;"/"&amp;E2</f>
         <v>TagGroup/cost-aexeo/BudgetCode/PROJECT-1212121</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>TagGroup/cost-aexeo/EBSCostCenter/4000009</v>
+        <v>TagGroup/cost-wan/BudgetCode/PROJECT-232222</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>TagGroup/cost-wan/BudgetCode/PROJECT-232222</v>
+        <v>TagGroup/sec-identity/BudgetCode/PROJECT-896775</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>TagGroup/cost-wan/EBSCostCenter/4000002</v>
+        <v>TagGroup/sec-threat/BudgetCode/PROJECT-901233</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>TagGroup/sec-identity/SecurityComponent/Identity</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>TagGroup/sec-threat/SecurityComponent/Threat</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>